<commit_message>
Agrego un módulo de búsqueda de precios, cargando un archivo de referencia.  Al tocar la X en la barra de búsqueda, el cursor se mete dentro de la barra automáticamente.
</commit_message>
<xml_diff>
--- a/data/Aumento_ofertas.xlsx
+++ b/data/Aumento_ofertas.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28816"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\working\waccache\CP1PEPF00001B92\EXCELCNV\f70b179d-6f18-45e1-bf60-b216ea87875a\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/1459e90a1e4def19/IT/Proyectos/2025 - Herramientas farmacia/precios_con_muebles/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2B72BCF7-9B5B-4F37-A11A-6F2E5F016EAA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="19" documentId="8_{2B72BCF7-9B5B-4F37-A11A-6F2E5F016EAA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9DAACB2B-A19F-49BD-9B81-AB24E96C65F9}"/>
   <bookViews>
-    <workbookView xWindow="-60" yWindow="-60" windowWidth="15480" windowHeight="11640" tabRatio="174" xr2:uid="{16DA3CDF-CF75-42A6-8E91-81DD33288EC1}"/>
+    <workbookView xWindow="1131" yWindow="1131" windowWidth="28003" windowHeight="15575" tabRatio="174" xr2:uid="{16DA3CDF-CF75-42A6-8E91-81DD33288EC1}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
     <t>Producto</t>
   </si>
@@ -49,21 +49,12 @@
     <t>Aludrox masticables x 3 blisters</t>
   </si>
   <si>
-    <t> $                      5.000</t>
-  </si>
-  <si>
     <t>Botiquín completo</t>
   </si>
   <si>
-    <t> $                    40.000</t>
-  </si>
-  <si>
     <t>Botiquín escuela</t>
   </si>
   <si>
-    <t> $                    30.000</t>
-  </si>
-  <si>
     <t>Botiquin familiar</t>
   </si>
   <si>
@@ -76,79 +67,43 @@
     <t>Crowie x 2</t>
   </si>
   <si>
-    <t> $                      1.000</t>
-  </si>
-  <si>
     <t>Guante x 10</t>
   </si>
   <si>
-    <t> $                      3.000</t>
-  </si>
-  <si>
     <t>Guantes x100 (caja)</t>
   </si>
   <si>
-    <t> $                    10.000</t>
-  </si>
-  <si>
     <t>Klonaprost</t>
   </si>
   <si>
-    <t> $                    17.000</t>
-  </si>
-  <si>
     <t>MASCARILLA FACIAL X 3</t>
   </si>
   <si>
-    <t> $                          400</t>
-  </si>
-  <si>
     <t>Metformina 500 x 30 x 2 blisters</t>
   </si>
   <si>
     <t>Metformina 850 x 30 x 2 blisters</t>
   </si>
   <si>
-    <t> $                    21.000</t>
-  </si>
-  <si>
     <t>Norviken K50 mgx 15 comp X2</t>
   </si>
   <si>
-    <t> $                      3.500</t>
-  </si>
-  <si>
     <t>Paño corporal x 10</t>
   </si>
   <si>
-    <t> $                      6.500</t>
-  </si>
-  <si>
     <t>Pañuelos de papel Sniff x10u X6</t>
   </si>
   <si>
     <t>NUEVAPINA X 7 BLISTER </t>
   </si>
   <si>
-    <t> $                      4.000</t>
-  </si>
-  <si>
     <t>NUEVAPINA X 4 BLISTER </t>
   </si>
   <si>
-    <t> $                      2.300</t>
-  </si>
-  <si>
     <t>ROSUVASTATINA 10 X 30 COMP - X 2 CAJAS</t>
   </si>
   <si>
-    <t> $                    28.000</t>
-  </si>
-  <si>
     <t>ATORVASTATINA 20 X 30 COMP - X 2 CAJAS</t>
-  </si>
-  <si>
-    <t> $                    50.000</t>
   </si>
 </sst>
 </file>
@@ -158,7 +113,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="dd/mm/yy"/>
   </numFmts>
-  <fonts count="2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -601,16 +556,16 @@
   <dimension ref="A1:C21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.53515625" defaultRowHeight="12.45" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="32.85546875" customWidth="1"/>
-    <col min="2" max="2" width="19.140625" customWidth="1"/>
+    <col min="1" max="1" width="32.84375" customWidth="1"/>
+    <col min="2" max="2" width="19.15234375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" ht="12.9" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -621,183 +576,183 @@
         <v>45772</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" ht="12.9" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="1">
+        <v>5000</v>
+      </c>
+      <c r="C2" s="3"/>
+    </row>
+    <row r="3" spans="1:3" ht="12.9" x14ac:dyDescent="0.35">
+      <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="3"/>
-    </row>
-    <row r="3" spans="1:3">
-      <c r="A3" s="1" t="s">
+      <c r="B3" s="1">
+        <v>40000</v>
+      </c>
+      <c r="C3" s="3"/>
+    </row>
+    <row r="4" spans="1:3" ht="12.9" x14ac:dyDescent="0.35">
+      <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B4" s="1">
+        <v>30000</v>
+      </c>
+      <c r="C4" s="3"/>
+    </row>
+    <row r="5" spans="1:3" ht="12.9" x14ac:dyDescent="0.35">
+      <c r="A5" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="3"/>
-    </row>
-    <row r="4" spans="1:3">
-      <c r="A4" s="1" t="s">
+      <c r="B5" s="1">
+        <v>30000</v>
+      </c>
+      <c r="C5" s="3"/>
+    </row>
+    <row r="6" spans="1:3" ht="12.9" x14ac:dyDescent="0.35">
+      <c r="A6" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B6" s="1">
+        <v>30000</v>
+      </c>
+      <c r="C6" s="3"/>
+    </row>
+    <row r="7" spans="1:3" ht="12.9" x14ac:dyDescent="0.35">
+      <c r="A7" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="3"/>
-    </row>
-    <row r="5" spans="1:3">
-      <c r="A5" s="1" t="s">
+      <c r="B7" s="1">
+        <v>30000</v>
+      </c>
+      <c r="C7" s="3"/>
+    </row>
+    <row r="8" spans="1:3" ht="12.9" x14ac:dyDescent="0.35">
+      <c r="A8" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C5" s="3"/>
-    </row>
-    <row r="6" spans="1:3">
-      <c r="A6" s="1" t="s">
+      <c r="B8" s="1">
+        <v>1000</v>
+      </c>
+      <c r="C8" s="3"/>
+    </row>
+    <row r="9" spans="1:3" ht="12.9" x14ac:dyDescent="0.35">
+      <c r="A9" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B6" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C6" s="3"/>
-    </row>
-    <row r="7" spans="1:3">
-      <c r="A7" s="1" t="s">
+      <c r="B9" s="1">
+        <v>3000</v>
+      </c>
+      <c r="C9" s="3"/>
+    </row>
+    <row r="10" spans="1:3" ht="12.9" x14ac:dyDescent="0.35">
+      <c r="A10" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B7" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C7" s="3"/>
-    </row>
-    <row r="8" spans="1:3">
-      <c r="A8" s="1" t="s">
+      <c r="B10" s="1">
+        <v>10000</v>
+      </c>
+      <c r="C10" s="3"/>
+    </row>
+    <row r="11" spans="1:3" ht="12.9" x14ac:dyDescent="0.35">
+      <c r="A11" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B11" s="1">
+        <v>17000</v>
+      </c>
+      <c r="C11" s="3"/>
+    </row>
+    <row r="12" spans="1:3" ht="12.9" x14ac:dyDescent="0.35">
+      <c r="A12" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C8" s="3"/>
-    </row>
-    <row r="9" spans="1:3">
-      <c r="A9" s="1" t="s">
+      <c r="B12" s="1">
+        <v>400</v>
+      </c>
+      <c r="C12" s="3"/>
+    </row>
+    <row r="13" spans="1:3" ht="12.9" x14ac:dyDescent="0.35">
+      <c r="A13" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="B13" s="1">
+        <v>10000</v>
+      </c>
+      <c r="C13" s="3"/>
+    </row>
+    <row r="14" spans="1:3" ht="12.9" x14ac:dyDescent="0.35">
+      <c r="A14" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C9" s="3"/>
-    </row>
-    <row r="10" spans="1:3">
-      <c r="A10" s="1" t="s">
+      <c r="B14" s="1">
+        <v>21000</v>
+      </c>
+      <c r="C14" s="3"/>
+    </row>
+    <row r="15" spans="1:3" ht="12.9" x14ac:dyDescent="0.35">
+      <c r="A15" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="B15" s="1">
+        <v>3500</v>
+      </c>
+      <c r="C15" s="3"/>
+    </row>
+    <row r="16" spans="1:3" ht="12.9" x14ac:dyDescent="0.35">
+      <c r="A16" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C10" s="3"/>
-    </row>
-    <row r="11" spans="1:3">
-      <c r="A11" s="1" t="s">
+      <c r="B16" s="1">
+        <v>6500</v>
+      </c>
+      <c r="C16" s="3"/>
+    </row>
+    <row r="17" spans="1:3" ht="12.9" x14ac:dyDescent="0.35">
+      <c r="A17" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="B17" s="1">
+        <v>3000</v>
+      </c>
+      <c r="C17" s="3"/>
+    </row>
+    <row r="18" spans="1:3" ht="12.9" x14ac:dyDescent="0.35">
+      <c r="A18" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C11" s="3"/>
-    </row>
-    <row r="12" spans="1:3">
-      <c r="A12" s="1" t="s">
+      <c r="B18" s="1">
+        <v>4000</v>
+      </c>
+      <c r="C18" s="3"/>
+    </row>
+    <row r="19" spans="1:3" ht="12.9" x14ac:dyDescent="0.35">
+      <c r="A19" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B12" s="1" t="s">
+      <c r="B19" s="1">
+        <v>2300</v>
+      </c>
+      <c r="C19" s="3"/>
+    </row>
+    <row r="20" spans="1:3" ht="25.75" x14ac:dyDescent="0.35">
+      <c r="A20" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C12" s="3"/>
-    </row>
-    <row r="13" spans="1:3">
-      <c r="A13" s="1" t="s">
+      <c r="B20" s="1">
+        <v>28000</v>
+      </c>
+      <c r="C20" s="3"/>
+    </row>
+    <row r="21" spans="1:3" ht="25.75" x14ac:dyDescent="0.35">
+      <c r="A21" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B13" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C13" s="3"/>
-    </row>
-    <row r="14" spans="1:3">
-      <c r="A14" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="C14" s="3"/>
-    </row>
-    <row r="15" spans="1:3">
-      <c r="A15" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C15" s="3"/>
-    </row>
-    <row r="16" spans="1:3">
-      <c r="A16" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="C16" s="3"/>
-    </row>
-    <row r="17" spans="1:3">
-      <c r="A17" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C17" s="3"/>
-    </row>
-    <row r="18" spans="1:3">
-      <c r="A18" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="C18" s="3"/>
-    </row>
-    <row r="19" spans="1:3">
-      <c r="A19" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="C19" s="3"/>
-    </row>
-    <row r="20" spans="1:3" ht="25.5">
-      <c r="A20" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="C20" s="3"/>
-    </row>
-    <row r="21" spans="1:3" ht="25.5">
-      <c r="A21" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>36</v>
+      <c r="B21" s="1">
+        <v>50000</v>
       </c>
     </row>
   </sheetData>
@@ -817,7 +772,7 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.53515625" defaultRowHeight="12.45" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.0527777777777778" bottom="1.0527777777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
@@ -835,7 +790,7 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.53515625" defaultRowHeight="12.45" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.0527777777777778" bottom="1.0527777777777778" header="0.78749999999999998" footer="0.78749999999999998"/>

</xml_diff>